<commit_message>
add compatibility with other resolutions, add 'close' hotkeys, add quick load on start screen
</commit_message>
<xml_diff>
--- a/MK_Hotkeys_Project_Design.xlsx
+++ b/MK_Hotkeys_Project_Design.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Positions" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Combinations" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="工作表3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="157">
   <si>
     <t xml:space="preserve">名称</t>
   </si>
@@ -200,6 +201,9 @@
     <t xml:space="preserve">sys_resume</t>
   </si>
   <si>
+    <t xml:space="preserve">!s</t>
+  </si>
+  <si>
     <t xml:space="preserve">离开</t>
   </si>
   <si>
@@ -266,6 +270,138 @@
     <t xml:space="preserve">sl_slot</t>
   </si>
   <si>
+    <t xml:space="preserve">子菜单</t>
+  </si>
+  <si>
+    <t xml:space="preserve">开始界面读取</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_start_load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">历史返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back_op_history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!F1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">分析返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back_op_analyze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!f2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">系统菜单返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">人物返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back_op_characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">建筑返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back_op_buildings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">交易返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back_op_market</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">移动返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back_op_move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">出击返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back_op_attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">侦察返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back_op_scout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">交涉返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back_op_negotiate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">情报返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back_op_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">任命返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back_op_assign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">传闻返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back_op_incident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">建筑物返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_back_building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">成果返回</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_back_fruit</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hotkey</t>
   </si>
   <si>
@@ -309,6 +445,54 @@
   </si>
   <si>
     <t xml:space="preserve">F4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">从各子界面返回经营界面</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comb_backs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_backs_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_backs_1, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_back_2, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_back_3, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_back_build, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_back_incident, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_back_char, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_back_building, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_back_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_back_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_back_build</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_back_incident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_back_char</t>
   </si>
 </sst>
 </file>
@@ -318,7 +502,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -344,13 +528,26 @@
       <family val="0"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE181E"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEF413D"/>
+        <bgColor rgb="FFCE181E"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -387,7 +584,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -400,6 +597,34 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -409,6 +634,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFEF413D"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -417,30 +702,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q2" activeCellId="1" sqref="I2:I5 Q2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P28" activeCellId="0" sqref="P28:P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="12.62"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="0" width="32.75"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="0" width="71.62"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="0" width="53.87"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="1" width="25.75"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="14" style="0" width="61.61"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="15" min="15" style="0" width="90.37"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="16" min="16" style="0" width="51.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="3.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="32.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="71.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="53.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="25.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="54.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="83.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="66.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -542,8 +829,8 @@
         <v>Iniread, k_op_history, .\config.ini, Keys, k_op_history</v>
       </c>
       <c r="O2" s="0" t="str">
-        <f aca="false">"click_abs_"&amp;D2&amp;" := Func(""to_click"").Bind(abs_"&amp;D2&amp;", , if_pos_res)"</f>
-        <v>click_abs_op_history := Func("to_click").Bind(abs_op_history, , if_pos_res)</v>
+        <f aca="false">"click_abs_"&amp;D2&amp;" := Func(""one_click"").Bind(abs_"&amp;D2&amp;", , if_pos_res)"</f>
+        <v>click_abs_op_history := Func("one_click").Bind(abs_op_history, , if_pos_res)</v>
       </c>
       <c r="P2" s="0" t="str">
         <f aca="false">"Hotkey, %k_"&amp;D2&amp;"%, % click_abs_"&amp;D2</f>
@@ -552,6 +839,10 @@
       <c r="Q2" s="0" t="str">
         <f aca="false">B2&amp;": %k_"&amp;D2&amp;"%"</f>
         <v>历史: %k_op_history%</v>
+      </c>
+      <c r="R2" s="0" t="str">
+        <f aca="false">"back_"&amp;D2</f>
+        <v>back_op_history</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -600,8 +891,8 @@
         <v>Iniread, k_op_analyze, .\config.ini, Keys, k_op_analyze</v>
       </c>
       <c r="O3" s="0" t="str">
-        <f aca="false">"click_abs_"&amp;D3&amp;" := Func(""to_click"").Bind(abs_"&amp;D3&amp;", , if_pos_res)"</f>
-        <v>click_abs_op_analyze := Func("to_click").Bind(abs_op_analyze, , if_pos_res)</v>
+        <f aca="false">"click_abs_"&amp;D3&amp;" := Func(""one_click"").Bind(abs_"&amp;D3&amp;", , if_pos_res)"</f>
+        <v>click_abs_op_analyze := Func("one_click").Bind(abs_op_analyze, , if_pos_res)</v>
       </c>
       <c r="P3" s="0" t="str">
         <f aca="false">"Hotkey, %k_"&amp;D3&amp;"%, % click_abs_"&amp;D3</f>
@@ -610,6 +901,10 @@
       <c r="Q3" s="0" t="str">
         <f aca="false">B3&amp;": %k_"&amp;D3&amp;"%"</f>
         <v>分析: %k_op_analyze%</v>
+      </c>
+      <c r="R3" s="0" t="str">
+        <f aca="false">"back_"&amp;D3</f>
+        <v>back_op_analyze</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -658,8 +953,8 @@
         <v>Iniread, k_op_system, .\config.ini, Keys, k_op_system</v>
       </c>
       <c r="O4" s="0" t="str">
-        <f aca="false">"click_abs_"&amp;D4&amp;" := Func(""to_click"").Bind(abs_"&amp;D4&amp;", , if_pos_res)"</f>
-        <v>click_abs_op_system := Func("to_click").Bind(abs_op_system, , if_pos_res)</v>
+        <f aca="false">"click_abs_"&amp;D4&amp;" := Func(""one_click"").Bind(abs_"&amp;D4&amp;", , if_pos_res)"</f>
+        <v>click_abs_op_system := Func("one_click").Bind(abs_op_system, , if_pos_res)</v>
       </c>
       <c r="P4" s="0" t="str">
         <f aca="false">"Hotkey, %k_"&amp;D4&amp;"%, % click_abs_"&amp;D4</f>
@@ -668,6 +963,10 @@
       <c r="Q4" s="0" t="str">
         <f aca="false">B4&amp;": %k_"&amp;D4&amp;"%"</f>
         <v>系统: %k_op_system%</v>
+      </c>
+      <c r="R4" s="0" t="str">
+        <f aca="false">"back_"&amp;D4</f>
+        <v>back_op_system</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -716,8 +1015,8 @@
         <v>Iniread, k_op_characters, .\config.ini, Keys, k_op_characters</v>
       </c>
       <c r="O5" s="0" t="str">
-        <f aca="false">"click_abs_"&amp;D5&amp;" := Func(""to_click"").Bind(abs_"&amp;D5&amp;", , if_pos_res)"</f>
-        <v>click_abs_op_characters := Func("to_click").Bind(abs_op_characters, , if_pos_res)</v>
+        <f aca="false">"click_abs_"&amp;D5&amp;" := Func(""one_click"").Bind(abs_"&amp;D5&amp;", , if_pos_res)"</f>
+        <v>click_abs_op_characters := Func("one_click").Bind(abs_op_characters, , if_pos_res)</v>
       </c>
       <c r="P5" s="0" t="str">
         <f aca="false">"Hotkey, %k_"&amp;D5&amp;"%, % click_abs_"&amp;D5</f>
@@ -726,6 +1025,10 @@
       <c r="Q5" s="0" t="str">
         <f aca="false">B5&amp;": %k_"&amp;D5&amp;"%"</f>
         <v>人物: %k_op_characters%</v>
+      </c>
+      <c r="R5" s="0" t="str">
+        <f aca="false">"back_"&amp;D5</f>
+        <v>back_op_characters</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -774,8 +1077,8 @@
         <v>Iniread, k_op_buildings, .\config.ini, Keys, k_op_buildings</v>
       </c>
       <c r="O6" s="0" t="str">
-        <f aca="false">"click_abs_"&amp;D6&amp;" := Func(""to_click"").Bind(abs_"&amp;D6&amp;", , if_pos_res)"</f>
-        <v>click_abs_op_buildings := Func("to_click").Bind(abs_op_buildings, , if_pos_res)</v>
+        <f aca="false">"click_abs_"&amp;D6&amp;" := Func(""one_click"").Bind(abs_"&amp;D6&amp;", , if_pos_res)"</f>
+        <v>click_abs_op_buildings := Func("one_click").Bind(abs_op_buildings, , if_pos_res)</v>
       </c>
       <c r="P6" s="0" t="str">
         <f aca="false">"Hotkey, %k_"&amp;D6&amp;"%, % click_abs_"&amp;D6</f>
@@ -784,6 +1087,10 @@
       <c r="Q6" s="0" t="str">
         <f aca="false">B6&amp;": %k_"&amp;D6&amp;"%"</f>
         <v>建筑: %k_op_buildings%</v>
+      </c>
+      <c r="R6" s="0" t="str">
+        <f aca="false">"back_"&amp;D6</f>
+        <v>back_op_buildings</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -832,8 +1139,8 @@
         <v>Iniread, k_op_market, .\config.ini, Keys, k_op_market</v>
       </c>
       <c r="O7" s="0" t="str">
-        <f aca="false">"click_abs_"&amp;D7&amp;" := Func(""to_click"").Bind(abs_"&amp;D7&amp;", , if_pos_res)"</f>
-        <v>click_abs_op_market := Func("to_click").Bind(abs_op_market, , if_pos_res)</v>
+        <f aca="false">"click_abs_"&amp;D7&amp;" := Func(""one_click"").Bind(abs_"&amp;D7&amp;", , if_pos_res)"</f>
+        <v>click_abs_op_market := Func("one_click").Bind(abs_op_market, , if_pos_res)</v>
       </c>
       <c r="P7" s="0" t="str">
         <f aca="false">"Hotkey, %k_"&amp;D7&amp;"%, % click_abs_"&amp;D7</f>
@@ -842,6 +1149,10 @@
       <c r="Q7" s="0" t="str">
         <f aca="false">B7&amp;": %k_"&amp;D7&amp;"%"</f>
         <v>交易: %k_op_market%</v>
+      </c>
+      <c r="R7" s="0" t="str">
+        <f aca="false">"back_"&amp;D7</f>
+        <v>back_op_market</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -890,8 +1201,8 @@
         <v>Iniread, k_op_move, .\config.ini, Keys, k_op_move</v>
       </c>
       <c r="O8" s="0" t="str">
-        <f aca="false">"click_abs_"&amp;D8&amp;" := Func(""to_click"").Bind(abs_"&amp;D8&amp;", , if_pos_res)"</f>
-        <v>click_abs_op_move := Func("to_click").Bind(abs_op_move, , if_pos_res)</v>
+        <f aca="false">"click_abs_"&amp;D8&amp;" := Func(""one_click"").Bind(abs_"&amp;D8&amp;", , if_pos_res)"</f>
+        <v>click_abs_op_move := Func("one_click").Bind(abs_op_move, , if_pos_res)</v>
       </c>
       <c r="P8" s="0" t="str">
         <f aca="false">"Hotkey, %k_"&amp;D8&amp;"%, % click_abs_"&amp;D8</f>
@@ -900,6 +1211,10 @@
       <c r="Q8" s="0" t="str">
         <f aca="false">B8&amp;": %k_"&amp;D8&amp;"%"</f>
         <v>移动: %k_op_move%</v>
+      </c>
+      <c r="R8" s="0" t="str">
+        <f aca="false">"back_"&amp;D8</f>
+        <v>back_op_move</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -948,8 +1263,8 @@
         <v>Iniread, k_op_attack, .\config.ini, Keys, k_op_attack</v>
       </c>
       <c r="O9" s="0" t="str">
-        <f aca="false">"click_abs_"&amp;D9&amp;" := Func(""to_click"").Bind(abs_"&amp;D9&amp;", , if_pos_res)"</f>
-        <v>click_abs_op_attack := Func("to_click").Bind(abs_op_attack, , if_pos_res)</v>
+        <f aca="false">"click_abs_"&amp;D9&amp;" := Func(""one_click"").Bind(abs_"&amp;D9&amp;", , if_pos_res)"</f>
+        <v>click_abs_op_attack := Func("one_click").Bind(abs_op_attack, , if_pos_res)</v>
       </c>
       <c r="P9" s="0" t="str">
         <f aca="false">"Hotkey, %k_"&amp;D9&amp;"%, % click_abs_"&amp;D9</f>
@@ -958,6 +1273,10 @@
       <c r="Q9" s="0" t="str">
         <f aca="false">B9&amp;": %k_"&amp;D9&amp;"%"</f>
         <v>出击: %k_op_attack%</v>
+      </c>
+      <c r="R9" s="0" t="str">
+        <f aca="false">"back_"&amp;D9</f>
+        <v>back_op_attack</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1006,8 +1325,8 @@
         <v>Iniread, k_op_scout, .\config.ini, Keys, k_op_scout</v>
       </c>
       <c r="O10" s="0" t="str">
-        <f aca="false">"click_abs_"&amp;D10&amp;" := Func(""to_click"").Bind(abs_"&amp;D10&amp;", , if_pos_res)"</f>
-        <v>click_abs_op_scout := Func("to_click").Bind(abs_op_scout, , if_pos_res)</v>
+        <f aca="false">"click_abs_"&amp;D10&amp;" := Func(""one_click"").Bind(abs_"&amp;D10&amp;", , if_pos_res)"</f>
+        <v>click_abs_op_scout := Func("one_click").Bind(abs_op_scout, , if_pos_res)</v>
       </c>
       <c r="P10" s="0" t="str">
         <f aca="false">"Hotkey, %k_"&amp;D10&amp;"%, % click_abs_"&amp;D10</f>
@@ -1016,6 +1335,10 @@
       <c r="Q10" s="0" t="str">
         <f aca="false">B10&amp;": %k_"&amp;D10&amp;"%"</f>
         <v>侦察: %k_op_scout%</v>
+      </c>
+      <c r="R10" s="0" t="str">
+        <f aca="false">"back_"&amp;D10</f>
+        <v>back_op_scout</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1064,8 +1387,8 @@
         <v>Iniread, k_op_negotiate, .\config.ini, Keys, k_op_negotiate</v>
       </c>
       <c r="O11" s="0" t="str">
-        <f aca="false">"click_abs_"&amp;D11&amp;" := Func(""to_click"").Bind(abs_"&amp;D11&amp;", , if_pos_res)"</f>
-        <v>click_abs_op_negotiate := Func("to_click").Bind(abs_op_negotiate, , if_pos_res)</v>
+        <f aca="false">"click_abs_"&amp;D11&amp;" := Func(""one_click"").Bind(abs_"&amp;D11&amp;", , if_pos_res)"</f>
+        <v>click_abs_op_negotiate := Func("one_click").Bind(abs_op_negotiate, , if_pos_res)</v>
       </c>
       <c r="P11" s="0" t="str">
         <f aca="false">"Hotkey, %k_"&amp;D11&amp;"%, % click_abs_"&amp;D11</f>
@@ -1074,6 +1397,10 @@
       <c r="Q11" s="0" t="str">
         <f aca="false">B11&amp;": %k_"&amp;D11&amp;"%"</f>
         <v>交涉: %k_op_negotiate%</v>
+      </c>
+      <c r="R11" s="0" t="str">
+        <f aca="false">"back_"&amp;D11</f>
+        <v>back_op_negotiate</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1122,8 +1449,8 @@
         <v>Iniread, k_op_info, .\config.ini, Keys, k_op_info</v>
       </c>
       <c r="O12" s="0" t="str">
-        <f aca="false">"click_abs_"&amp;D12&amp;" := Func(""to_click"").Bind(abs_"&amp;D12&amp;", , if_pos_res)"</f>
-        <v>click_abs_op_info := Func("to_click").Bind(abs_op_info, , if_pos_res)</v>
+        <f aca="false">"click_abs_"&amp;D12&amp;" := Func(""one_click"").Bind(abs_"&amp;D12&amp;", , if_pos_res)"</f>
+        <v>click_abs_op_info := Func("one_click").Bind(abs_op_info, , if_pos_res)</v>
       </c>
       <c r="P12" s="0" t="str">
         <f aca="false">"Hotkey, %k_"&amp;D12&amp;"%, % click_abs_"&amp;D12</f>
@@ -1132,6 +1459,10 @@
       <c r="Q12" s="0" t="str">
         <f aca="false">B12&amp;": %k_"&amp;D12&amp;"%"</f>
         <v>情报: %k_op_info%</v>
+      </c>
+      <c r="R12" s="0" t="str">
+        <f aca="false">"back_"&amp;D12</f>
+        <v>back_op_info</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1180,8 +1511,8 @@
         <v>Iniread, k_op_assign, .\config.ini, Keys, k_op_assign</v>
       </c>
       <c r="O13" s="0" t="str">
-        <f aca="false">"click_abs_"&amp;D13&amp;" := Func(""to_click"").Bind(abs_"&amp;D13&amp;", , if_pos_res)"</f>
-        <v>click_abs_op_assign := Func("to_click").Bind(abs_op_assign, , if_pos_res)</v>
+        <f aca="false">"click_abs_"&amp;D13&amp;" := Func(""one_click"").Bind(abs_"&amp;D13&amp;", , if_pos_res)"</f>
+        <v>click_abs_op_assign := Func("one_click").Bind(abs_op_assign, , if_pos_res)</v>
       </c>
       <c r="P13" s="0" t="str">
         <f aca="false">"Hotkey, %k_"&amp;D13&amp;"%, % click_abs_"&amp;D13</f>
@@ -1190,6 +1521,10 @@
       <c r="Q13" s="0" t="str">
         <f aca="false">B13&amp;": %k_"&amp;D13&amp;"%"</f>
         <v>任命: %k_op_assign%</v>
+      </c>
+      <c r="R13" s="0" t="str">
+        <f aca="false">"back_"&amp;D13</f>
+        <v>back_op_assign</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1238,13 +1573,17 @@
         <v>Iniread, k_op_incident, .\config.ini, Keys, k_op_incident</v>
       </c>
       <c r="O14" s="0" t="str">
-        <f aca="false">"click_abs_"&amp;D14&amp;" := Func(""to_click"").Bind(abs_"&amp;D14&amp;", , if_pos_res)"</f>
-        <v>click_abs_op_incident := Func("to_click").Bind(abs_op_incident, , if_pos_res)</v>
+        <f aca="false">"click_abs_"&amp;D14&amp;" := Func(""one_click"").Bind(abs_"&amp;D14&amp;", , if_pos_res)"</f>
+        <v>click_abs_op_incident := Func("one_click").Bind(abs_op_incident, , if_pos_res)</v>
       </c>
       <c r="P14" s="0" t="str">
         <f aca="false">"Hotkey, %k_"&amp;D14&amp;"%, % click_abs_"&amp;D14</f>
         <v>Hotkey, %k_op_incident%, % click_abs_op_incident</v>
       </c>
+      <c r="R14" s="0" t="str">
+        <f aca="false">"back_"&amp;D14</f>
+        <v>back_op_incident</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -1318,11 +1657,14 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>58</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>400</v>
@@ -1353,10 +1695,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>400</v>
@@ -1387,10 +1729,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>397</v>
@@ -1421,10 +1763,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>470</v>
@@ -1455,10 +1797,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>379</v>
@@ -1489,13 +1831,13 @@
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>368</v>
@@ -1526,13 +1868,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>429</v>
@@ -1563,16 +1905,16 @@
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>370</v>
@@ -1603,13 +1945,13 @@
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>433</v>
@@ -1640,13 +1982,13 @@
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>400</v>
@@ -1675,6 +2017,762 @@
         <v>abs_sl_slot := find_pos(sl_slot)</v>
       </c>
     </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>482</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>322</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <f aca="false">ROUND(F27/800,4)</f>
+        <v>0.6025</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <f aca="false">ROUND(G27/600,4)</f>
+        <v>0.5367</v>
+      </c>
+      <c r="J27" s="0" t="str">
+        <f aca="false">D27&amp;"="&amp;H27&amp;","&amp;I27</f>
+        <v>sub_start_load=0.6025,0.5367</v>
+      </c>
+      <c r="K27" s="2" t="str">
+        <f aca="false">"IniRead, "&amp;D27&amp;", .\config.ini, Proportions, "&amp;D27</f>
+        <v>IniRead, sub_start_load, .\config.ini, Proportions, sub_start_load</v>
+      </c>
+      <c r="L27" s="2" t="str">
+        <f aca="false">"abs_"&amp;D27&amp;" := find_pos("&amp;D27&amp;")"</f>
+        <v>abs_sub_start_load := find_pos(sub_start_load)</v>
+      </c>
+    </row>
+    <row r="28" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" s="4" t="n">
+        <v>400</v>
+      </c>
+      <c r="G28" s="4" t="n">
+        <v>566</v>
+      </c>
+      <c r="H28" s="4" t="n">
+        <f aca="false">ROUND(F28/800,4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I28" s="4" t="n">
+        <f aca="false">ROUND(G28/600,4)</f>
+        <v>0.9433</v>
+      </c>
+      <c r="J28" s="4" t="str">
+        <f aca="false">D28&amp;"="&amp;H28&amp;","&amp;I28</f>
+        <v>back_op_history=0.5,0.9433</v>
+      </c>
+      <c r="K28" s="5" t="str">
+        <f aca="false">"IniRead, "&amp;D28&amp;", .\config.ini, Proportions, "&amp;D28</f>
+        <v>IniRead, back_op_history, .\config.ini, Proportions, back_op_history</v>
+      </c>
+      <c r="L28" s="5" t="str">
+        <f aca="false">"abs_"&amp;D28&amp;" := find_pos("&amp;D28&amp;")"</f>
+        <v>abs_back_op_history := find_pos(back_op_history)</v>
+      </c>
+      <c r="M28" s="6"/>
+      <c r="N28" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="O28" s="0" t="str">
+        <f aca="false">"click_abs_"&amp;D28&amp;" := Func(""one_click"").Bind(abs_"&amp;D28&amp;", , if_pos_res)"</f>
+        <v>click_abs_back_op_history := Func("one_click").Bind(abs_back_op_history, , if_pos_res)</v>
+      </c>
+      <c r="P28" s="0" t="str">
+        <f aca="false">"Hotkey, %k_op_backs%%k_"&amp;N28&amp;"%, % click_abs_"&amp;D28</f>
+        <v>Hotkey, %k_op_backs%%k_op_history%, % click_abs_back_op_history</v>
+      </c>
+    </row>
+    <row r="29" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="4" t="n">
+        <v>400</v>
+      </c>
+      <c r="G29" s="4" t="n">
+        <v>566</v>
+      </c>
+      <c r="H29" s="4" t="n">
+        <f aca="false">ROUND(F29/800,4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I29" s="4" t="n">
+        <f aca="false">ROUND(G29/600,4)</f>
+        <v>0.9433</v>
+      </c>
+      <c r="J29" s="4" t="str">
+        <f aca="false">D29&amp;"="&amp;H29&amp;","&amp;I29</f>
+        <v>back_op_analyze=0.5,0.9433</v>
+      </c>
+      <c r="K29" s="5" t="str">
+        <f aca="false">"IniRead, "&amp;D29&amp;", .\config.ini, Proportions, "&amp;D29</f>
+        <v>IniRead, back_op_analyze, .\config.ini, Proportions, back_op_analyze</v>
+      </c>
+      <c r="L29" s="5" t="str">
+        <f aca="false">"abs_"&amp;D29&amp;" := find_pos("&amp;D29&amp;")"</f>
+        <v>abs_back_op_analyze := find_pos(back_op_analyze)</v>
+      </c>
+      <c r="M29" s="6"/>
+      <c r="N29" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="O29" s="0" t="str">
+        <f aca="false">"click_abs_"&amp;D29&amp;" := Func(""one_click"").Bind(abs_"&amp;D29&amp;", , if_pos_res)"</f>
+        <v>click_abs_back_op_analyze := Func("one_click").Bind(abs_back_op_analyze, , if_pos_res)</v>
+      </c>
+      <c r="P29" s="0" t="str">
+        <f aca="false">"Hotkey, %k_op_backs%%k_"&amp;N29&amp;"%, % click_abs_"&amp;D29</f>
+        <v>Hotkey, %k_op_backs%%k_op_analyze%, % click_abs_back_op_analyze</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>440</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <f aca="false">ROUND(F30/800,4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <f aca="false">ROUND(G30/600,4)</f>
+        <v>0.7333</v>
+      </c>
+      <c r="J30" s="0" t="str">
+        <f aca="false">D30&amp;"="&amp;H30&amp;","&amp;I30</f>
+        <v>sys_resume=0.5,0.7333</v>
+      </c>
+      <c r="K30" s="2" t="str">
+        <f aca="false">"IniRead, "&amp;D30&amp;", .\config.ini, Proportions, "&amp;D30</f>
+        <v>IniRead, sys_resume, .\config.ini, Proportions, sys_resume</v>
+      </c>
+      <c r="L30" s="2" t="str">
+        <f aca="false">"abs_"&amp;D30&amp;" := find_pos("&amp;D30&amp;")"</f>
+        <v>abs_sys_resume := find_pos(sys_resume)</v>
+      </c>
+      <c r="N30" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O30" s="0" t="str">
+        <f aca="false">"click_abs_"&amp;D30&amp;" := Func(""one_click"").Bind(abs_"&amp;D30&amp;", , if_pos_res)"</f>
+        <v>click_abs_sys_resume := Func("one_click").Bind(abs_sys_resume, , if_pos_res)</v>
+      </c>
+      <c r="P30" s="0" t="str">
+        <f aca="false">"Hotkey, %k_op_backs%%k_"&amp;N30&amp;"%, % click_abs_"&amp;D30</f>
+        <v>Hotkey, %k_op_backs%%k_op_system%, % click_abs_sys_resume</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>552</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>490</v>
+      </c>
+      <c r="H31" s="4" t="n">
+        <f aca="false">ROUND(F31/800,4)</f>
+        <v>0.69</v>
+      </c>
+      <c r="I31" s="4" t="n">
+        <f aca="false">ROUND(G31/600,4)</f>
+        <v>0.8167</v>
+      </c>
+      <c r="J31" s="4" t="str">
+        <f aca="false">D31&amp;"="&amp;H31&amp;","&amp;I31</f>
+        <v>back_op_characters=0.69,0.8167</v>
+      </c>
+      <c r="K31" s="5" t="str">
+        <f aca="false">"IniRead, "&amp;D31&amp;", .\config.ini, Proportions, "&amp;D31</f>
+        <v>IniRead, back_op_characters, .\config.ini, Proportions, back_op_characters</v>
+      </c>
+      <c r="L31" s="5" t="str">
+        <f aca="false">"abs_"&amp;D31&amp;" := find_pos("&amp;D31&amp;")"</f>
+        <v>abs_back_op_characters := find_pos(back_op_characters)</v>
+      </c>
+      <c r="N31" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O31" s="0" t="str">
+        <f aca="false">"click_abs_"&amp;D31&amp;" := Func(""one_click"").Bind(abs_"&amp;D31&amp;", , if_pos_res)"</f>
+        <v>click_abs_back_op_characters := Func("one_click").Bind(abs_back_op_characters, , if_pos_res)</v>
+      </c>
+      <c r="P31" s="0" t="str">
+        <f aca="false">"Hotkey, %k_op_backs%%k_"&amp;N31&amp;"%, % click_abs_"&amp;D31</f>
+        <v>Hotkey, %k_op_backs%%k_op_characters%, % click_abs_back_op_characters</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>442</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>441</v>
+      </c>
+      <c r="H32" s="4" t="n">
+        <f aca="false">ROUND(F32/800,4)</f>
+        <v>0.5525</v>
+      </c>
+      <c r="I32" s="4" t="n">
+        <f aca="false">ROUND(G32/600,4)</f>
+        <v>0.735</v>
+      </c>
+      <c r="J32" s="4" t="str">
+        <f aca="false">D32&amp;"="&amp;H32&amp;","&amp;I32</f>
+        <v>back_op_buildings=0.5525,0.735</v>
+      </c>
+      <c r="K32" s="5" t="str">
+        <f aca="false">"IniRead, "&amp;D32&amp;", .\config.ini, Proportions, "&amp;D32</f>
+        <v>IniRead, back_op_buildings, .\config.ini, Proportions, back_op_buildings</v>
+      </c>
+      <c r="L32" s="5" t="str">
+        <f aca="false">"abs_"&amp;D32&amp;" := find_pos("&amp;D32&amp;")"</f>
+        <v>abs_back_op_buildings := find_pos(back_op_buildings)</v>
+      </c>
+      <c r="N32" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O32" s="0" t="str">
+        <f aca="false">"click_abs_"&amp;D32&amp;" := Func(""one_click"").Bind(abs_"&amp;D32&amp;", , if_pos_res)"</f>
+        <v>click_abs_back_op_buildings := Func("one_click").Bind(abs_back_op_buildings, , if_pos_res)</v>
+      </c>
+      <c r="P32" s="0" t="str">
+        <f aca="false">"Hotkey, %k_op_backs%%k_"&amp;N32&amp;"%, % click_abs_"&amp;D32</f>
+        <v>Hotkey, %k_op_backs%%k_op_buildings%, % click_abs_back_op_buildings</v>
+      </c>
+    </row>
+    <row r="33" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="4" t="n">
+        <v>400</v>
+      </c>
+      <c r="G33" s="4" t="n">
+        <v>566</v>
+      </c>
+      <c r="H33" s="4" t="n">
+        <f aca="false">ROUND(F33/800,4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I33" s="4" t="n">
+        <f aca="false">ROUND(G33/600,4)</f>
+        <v>0.9433</v>
+      </c>
+      <c r="J33" s="4" t="str">
+        <f aca="false">D33&amp;"="&amp;H33&amp;","&amp;I33</f>
+        <v>back_op_market=0.5,0.9433</v>
+      </c>
+      <c r="K33" s="5" t="str">
+        <f aca="false">"IniRead, "&amp;D33&amp;", .\config.ini, Proportions, "&amp;D33</f>
+        <v>IniRead, back_op_market, .\config.ini, Proportions, back_op_market</v>
+      </c>
+      <c r="L33" s="5" t="str">
+        <f aca="false">"abs_"&amp;D33&amp;" := find_pos("&amp;D33&amp;")"</f>
+        <v>abs_back_op_market := find_pos(back_op_market)</v>
+      </c>
+      <c r="M33" s="6"/>
+      <c r="N33" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="O33" s="0" t="str">
+        <f aca="false">"click_abs_"&amp;D33&amp;" := Func(""one_click"").Bind(abs_"&amp;D33&amp;", , if_pos_res)"</f>
+        <v>click_abs_back_op_market := Func("one_click").Bind(abs_back_op_market, , if_pos_res)</v>
+      </c>
+      <c r="P33" s="0" t="str">
+        <f aca="false">"Hotkey, %k_op_backs%%k_"&amp;N33&amp;"%, % click_abs_"&amp;D33</f>
+        <v>Hotkey, %k_op_backs%%k_op_market%, % click_abs_back_op_market</v>
+      </c>
+    </row>
+    <row r="34" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F34" s="4" t="n">
+        <v>485</v>
+      </c>
+      <c r="G34" s="4" t="n">
+        <v>522</v>
+      </c>
+      <c r="H34" s="4" t="n">
+        <f aca="false">ROUND(F34/800,4)</f>
+        <v>0.6063</v>
+      </c>
+      <c r="I34" s="4" t="n">
+        <f aca="false">ROUND(G34/600,4)</f>
+        <v>0.87</v>
+      </c>
+      <c r="J34" s="4" t="str">
+        <f aca="false">D34&amp;"="&amp;H34&amp;","&amp;I34</f>
+        <v>back_op_move=0.6063,0.87</v>
+      </c>
+      <c r="K34" s="5" t="str">
+        <f aca="false">"IniRead, "&amp;D34&amp;", .\config.ini, Proportions, "&amp;D34</f>
+        <v>IniRead, back_op_move, .\config.ini, Proportions, back_op_move</v>
+      </c>
+      <c r="L34" s="5" t="str">
+        <f aca="false">"abs_"&amp;D34&amp;" := find_pos("&amp;D34&amp;")"</f>
+        <v>abs_back_op_move := find_pos(back_op_move)</v>
+      </c>
+      <c r="M34" s="6"/>
+      <c r="N34" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O34" s="0" t="str">
+        <f aca="false">"click_abs_"&amp;D34&amp;" := Func(""one_click"").Bind(abs_"&amp;D34&amp;", , if_pos_res)"</f>
+        <v>click_abs_back_op_move := Func("one_click").Bind(abs_back_op_move, , if_pos_res)</v>
+      </c>
+      <c r="P34" s="0" t="str">
+        <f aca="false">"Hotkey, %k_op_backs%%k_"&amp;N34&amp;"%, % click_abs_"&amp;D34</f>
+        <v>Hotkey, %k_op_backs%%k_op_move%, % click_abs_back_op_move</v>
+      </c>
+    </row>
+    <row r="35" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F35" s="4" t="n">
+        <v>485</v>
+      </c>
+      <c r="G35" s="4" t="n">
+        <v>522</v>
+      </c>
+      <c r="H35" s="4" t="n">
+        <f aca="false">ROUND(F35/800,4)</f>
+        <v>0.6063</v>
+      </c>
+      <c r="I35" s="4" t="n">
+        <f aca="false">ROUND(G35/600,4)</f>
+        <v>0.87</v>
+      </c>
+      <c r="J35" s="4" t="str">
+        <f aca="false">D35&amp;"="&amp;H35&amp;","&amp;I35</f>
+        <v>back_op_attack=0.6063,0.87</v>
+      </c>
+      <c r="K35" s="5" t="str">
+        <f aca="false">"IniRead, "&amp;D35&amp;", .\config.ini, Proportions, "&amp;D35</f>
+        <v>IniRead, back_op_attack, .\config.ini, Proportions, back_op_attack</v>
+      </c>
+      <c r="L35" s="5" t="str">
+        <f aca="false">"abs_"&amp;D35&amp;" := find_pos("&amp;D35&amp;")"</f>
+        <v>abs_back_op_attack := find_pos(back_op_attack)</v>
+      </c>
+      <c r="M35" s="6"/>
+      <c r="N35" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O35" s="0" t="str">
+        <f aca="false">"click_abs_"&amp;D35&amp;" := Func(""one_click"").Bind(abs_"&amp;D35&amp;", , if_pos_res)"</f>
+        <v>click_abs_back_op_attack := Func("one_click").Bind(abs_back_op_attack, , if_pos_res)</v>
+      </c>
+      <c r="P35" s="0" t="str">
+        <f aca="false">"Hotkey, %k_op_backs%%k_"&amp;N35&amp;"%, % click_abs_"&amp;D35</f>
+        <v>Hotkey, %k_op_backs%%k_op_attack%, % click_abs_back_op_attack</v>
+      </c>
+    </row>
+    <row r="36" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36" s="4" t="n">
+        <v>485</v>
+      </c>
+      <c r="G36" s="4" t="n">
+        <v>522</v>
+      </c>
+      <c r="H36" s="4" t="n">
+        <f aca="false">ROUND(F36/800,4)</f>
+        <v>0.6063</v>
+      </c>
+      <c r="I36" s="4" t="n">
+        <f aca="false">ROUND(G36/600,4)</f>
+        <v>0.87</v>
+      </c>
+      <c r="J36" s="4" t="str">
+        <f aca="false">D36&amp;"="&amp;H36&amp;","&amp;I36</f>
+        <v>back_op_scout=0.6063,0.87</v>
+      </c>
+      <c r="K36" s="5" t="str">
+        <f aca="false">"IniRead, "&amp;D36&amp;", .\config.ini, Proportions, "&amp;D36</f>
+        <v>IniRead, back_op_scout, .\config.ini, Proportions, back_op_scout</v>
+      </c>
+      <c r="L36" s="5" t="str">
+        <f aca="false">"abs_"&amp;D36&amp;" := find_pos("&amp;D36&amp;")"</f>
+        <v>abs_back_op_scout := find_pos(back_op_scout)</v>
+      </c>
+      <c r="M36" s="6"/>
+      <c r="N36" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O36" s="0" t="str">
+        <f aca="false">"click_abs_"&amp;D36&amp;" := Func(""one_click"").Bind(abs_"&amp;D36&amp;", , if_pos_res)"</f>
+        <v>click_abs_back_op_scout := Func("one_click").Bind(abs_back_op_scout, , if_pos_res)</v>
+      </c>
+      <c r="P36" s="0" t="str">
+        <f aca="false">"Hotkey, %k_op_backs%%k_"&amp;N36&amp;"%, % click_abs_"&amp;D36</f>
+        <v>Hotkey, %k_op_backs%%k_op_scout%, % click_abs_back_op_scout</v>
+      </c>
+    </row>
+    <row r="37" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F37" s="4" t="n">
+        <v>485</v>
+      </c>
+      <c r="G37" s="4" t="n">
+        <v>522</v>
+      </c>
+      <c r="H37" s="4" t="n">
+        <f aca="false">ROUND(F37/800,4)</f>
+        <v>0.6063</v>
+      </c>
+      <c r="I37" s="4" t="n">
+        <f aca="false">ROUND(G37/600,4)</f>
+        <v>0.87</v>
+      </c>
+      <c r="J37" s="4" t="str">
+        <f aca="false">D37&amp;"="&amp;H37&amp;","&amp;I37</f>
+        <v>back_op_negotiate=0.6063,0.87</v>
+      </c>
+      <c r="K37" s="5" t="str">
+        <f aca="false">"IniRead, "&amp;D37&amp;", .\config.ini, Proportions, "&amp;D37</f>
+        <v>IniRead, back_op_negotiate, .\config.ini, Proportions, back_op_negotiate</v>
+      </c>
+      <c r="L37" s="5" t="str">
+        <f aca="false">"abs_"&amp;D37&amp;" := find_pos("&amp;D37&amp;")"</f>
+        <v>abs_back_op_negotiate := find_pos(back_op_negotiate)</v>
+      </c>
+      <c r="M37" s="6"/>
+      <c r="N37" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="O37" s="0" t="str">
+        <f aca="false">"click_abs_"&amp;D37&amp;" := Func(""one_click"").Bind(abs_"&amp;D37&amp;", , if_pos_res)"</f>
+        <v>click_abs_back_op_negotiate := Func("one_click").Bind(abs_back_op_negotiate, , if_pos_res)</v>
+      </c>
+      <c r="P37" s="0" t="str">
+        <f aca="false">"Hotkey, %k_op_backs%%k_"&amp;N37&amp;"%, % click_abs_"&amp;D37</f>
+        <v>Hotkey, %k_op_backs%%k_op_negotiate%, % click_abs_back_op_negotiate</v>
+      </c>
+    </row>
+    <row r="38" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="4" t="n">
+        <v>400</v>
+      </c>
+      <c r="G38" s="4" t="n">
+        <v>508</v>
+      </c>
+      <c r="H38" s="4" t="n">
+        <f aca="false">ROUND(F38/800,4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I38" s="4" t="n">
+        <f aca="false">ROUND(G38/600,4)</f>
+        <v>0.8467</v>
+      </c>
+      <c r="J38" s="4" t="str">
+        <f aca="false">D38&amp;"="&amp;H38&amp;","&amp;I38</f>
+        <v>back_op_info=0.5,0.8467</v>
+      </c>
+      <c r="K38" s="5" t="str">
+        <f aca="false">"IniRead, "&amp;D38&amp;", .\config.ini, Proportions, "&amp;D38</f>
+        <v>IniRead, back_op_info, .\config.ini, Proportions, back_op_info</v>
+      </c>
+      <c r="L38" s="5" t="str">
+        <f aca="false">"abs_"&amp;D38&amp;" := find_pos("&amp;D38&amp;")"</f>
+        <v>abs_back_op_info := find_pos(back_op_info)</v>
+      </c>
+      <c r="M38" s="6"/>
+      <c r="N38" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="O38" s="0" t="str">
+        <f aca="false">"click_abs_"&amp;D38&amp;" := Func(""one_click"").Bind(abs_"&amp;D38&amp;", , if_pos_res)"</f>
+        <v>click_abs_back_op_info := Func("one_click").Bind(abs_back_op_info, , if_pos_res)</v>
+      </c>
+      <c r="P38" s="0" t="str">
+        <f aca="false">"Hotkey, %k_op_backs%%k_"&amp;N38&amp;"%, % click_abs_"&amp;D38</f>
+        <v>Hotkey, %k_op_backs%%k_op_info%, % click_abs_back_op_info</v>
+      </c>
+    </row>
+    <row r="39" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F39" s="4" t="n">
+        <v>400</v>
+      </c>
+      <c r="G39" s="4" t="n">
+        <v>566</v>
+      </c>
+      <c r="H39" s="4" t="n">
+        <f aca="false">ROUND(F39/800,4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I39" s="4" t="n">
+        <f aca="false">ROUND(G39/600,4)</f>
+        <v>0.9433</v>
+      </c>
+      <c r="J39" s="4" t="str">
+        <f aca="false">D39&amp;"="&amp;H39&amp;","&amp;I39</f>
+        <v>back_op_assign=0.5,0.9433</v>
+      </c>
+      <c r="K39" s="5" t="str">
+        <f aca="false">"IniRead, "&amp;D39&amp;", .\config.ini, Proportions, "&amp;D39</f>
+        <v>IniRead, back_op_assign, .\config.ini, Proportions, back_op_assign</v>
+      </c>
+      <c r="L39" s="5" t="str">
+        <f aca="false">"abs_"&amp;D39&amp;" := find_pos("&amp;D39&amp;")"</f>
+        <v>abs_back_op_assign := find_pos(back_op_assign)</v>
+      </c>
+      <c r="M39" s="6"/>
+      <c r="N39" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="O39" s="0" t="str">
+        <f aca="false">"click_abs_"&amp;D39&amp;" := Func(""one_click"").Bind(abs_"&amp;D39&amp;", , if_pos_res)"</f>
+        <v>click_abs_back_op_assign := Func("one_click").Bind(abs_back_op_assign, , if_pos_res)</v>
+      </c>
+      <c r="P39" s="0" t="str">
+        <f aca="false">"Hotkey, %k_op_backs%%k_"&amp;N39&amp;"%, % click_abs_"&amp;D39</f>
+        <v>Hotkey, %k_op_backs%%k_op_assign%, % click_abs_back_op_assign</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>434</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>406</v>
+      </c>
+      <c r="H40" s="4" t="n">
+        <f aca="false">ROUND(F40/800,4)</f>
+        <v>0.5425</v>
+      </c>
+      <c r="I40" s="4" t="n">
+        <f aca="false">ROUND(G40/600,4)</f>
+        <v>0.6767</v>
+      </c>
+      <c r="J40" s="4" t="str">
+        <f aca="false">D40&amp;"="&amp;H40&amp;","&amp;I40</f>
+        <v>back_op_incident=0.5425,0.6767</v>
+      </c>
+      <c r="K40" s="5" t="str">
+        <f aca="false">"IniRead, "&amp;D40&amp;", .\config.ini, Proportions, "&amp;D40</f>
+        <v>IniRead, back_op_incident, .\config.ini, Proportions, back_op_incident</v>
+      </c>
+      <c r="L40" s="5" t="str">
+        <f aca="false">"abs_"&amp;D40&amp;" := find_pos("&amp;D40&amp;")"</f>
+        <v>abs_back_op_incident := find_pos(back_op_incident)</v>
+      </c>
+      <c r="N40" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="O40" s="0" t="str">
+        <f aca="false">"click_abs_"&amp;D40&amp;" := Func(""one_click"").Bind(abs_"&amp;D40&amp;", , if_pos_res)"</f>
+        <v>click_abs_back_op_incident := Func("one_click").Bind(abs_back_op_incident, , if_pos_res)</v>
+      </c>
+      <c r="P40" s="0" t="str">
+        <f aca="false">"Hotkey, %k_op_backs%%k_"&amp;N40&amp;"%, % click_abs_"&amp;D40</f>
+        <v>Hotkey, %k_op_backs%%k_op_incident%, % click_abs_back_op_incident</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>476</v>
+      </c>
+      <c r="H46" s="4" t="n">
+        <f aca="false">ROUND(F46/800,4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I46" s="4" t="n">
+        <f aca="false">ROUND(G46/600,4)</f>
+        <v>0.7933</v>
+      </c>
+      <c r="J46" s="4" t="str">
+        <f aca="false">D46&amp;"="&amp;H46&amp;","&amp;I46</f>
+        <v>sub_back_building=0.5,0.7933</v>
+      </c>
+      <c r="K46" s="5" t="str">
+        <f aca="false">"IniRead, "&amp;D46&amp;", .\config.ini, Proportions, "&amp;D46</f>
+        <v>IniRead, sub_back_building, .\config.ini, Proportions, sub_back_building</v>
+      </c>
+      <c r="L46" s="5" t="str">
+        <f aca="false">"abs_"&amp;D46&amp;" := find_pos("&amp;D46&amp;")"</f>
+        <v>abs_sub_back_building := find_pos(sub_back_building)</v>
+      </c>
+    </row>
+    <row r="47" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F47" s="4" t="n">
+        <v>400</v>
+      </c>
+      <c r="G47" s="4" t="n">
+        <v>508</v>
+      </c>
+      <c r="H47" s="4" t="n">
+        <f aca="false">ROUND(F47/800,4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I47" s="4" t="n">
+        <f aca="false">ROUND(G47/600,4)</f>
+        <v>0.8467</v>
+      </c>
+      <c r="J47" s="4" t="str">
+        <f aca="false">D47&amp;"="&amp;H47&amp;","&amp;I47</f>
+        <v>sub_back_fruit=0.5,0.8467</v>
+      </c>
+      <c r="K47" s="5" t="str">
+        <f aca="false">"IniRead, "&amp;D47&amp;", .\config.ini, Proportions, "&amp;D47</f>
+        <v>IniRead, sub_back_fruit, .\config.ini, Proportions, sub_back_fruit</v>
+      </c>
+      <c r="L47" s="5" t="str">
+        <f aca="false">"abs_"&amp;D47&amp;" := find_pos("&amp;D47&amp;")"</f>
+        <v>abs_sub_back_fruit := find_pos(sub_back_fruit)</v>
+      </c>
+      <c r="M47" s="6"/>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1691,22 +2789,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2:I5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="P28:P40 B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.65"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="1" width="22.75"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="56.76"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="7" min="7" style="0" width="68.71"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="8" style="0" width="48.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="56.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="68.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="48.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.65"/>
   </cols>
@@ -1722,7 +2820,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -1742,16 +2840,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="E2" s="1" t="str">
         <f aca="false">"k_"&amp;C2&amp;"="&amp;D2</f>
@@ -1776,16 +2874,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
       <c r="E3" s="1" t="str">
         <f aca="false">"k_"&amp;C3&amp;"="&amp;D3</f>
@@ -1810,16 +2908,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
       <c r="E4" s="1" t="str">
         <f aca="false">"k_"&amp;C4&amp;"="&amp;D4</f>
@@ -1844,16 +2942,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="E5" s="1" t="str">
         <f aca="false">"k_"&amp;C5&amp;"="&amp;D5</f>
@@ -1874,6 +2972,40 @@
       <c r="I5" s="0" t="str">
         <f aca="false">B5&amp;": %k_"&amp;C5&amp;"%"</f>
         <v>快速读取: %k_comb_quick_load%</v>
+      </c>
+    </row>
+    <row r="6" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="9" t="str">
+        <f aca="false">"k_"&amp;C6&amp;"="&amp;D6</f>
+        <v>k_comb_backs=Esc</v>
+      </c>
+      <c r="F6" s="8" t="str">
+        <f aca="false">"Iniread, k_"&amp;C6&amp;", .\config.ini, Keys, k_"&amp;C6</f>
+        <v>Iniread, k_comb_backs, .\config.ini, Keys, k_comb_backs</v>
+      </c>
+      <c r="G6" s="8" t="str">
+        <f aca="false">"click_"&amp;C6&amp;" := Func(""multi_clicks"").Bind("&amp;C6&amp;", if_pos_res)"</f>
+        <v>click_comb_backs := Func("multi_clicks").Bind(comb_backs, if_pos_res)</v>
+      </c>
+      <c r="H6" s="8" t="str">
+        <f aca="false">"Hotkey, %k_"&amp;C6&amp;"%, % click_"&amp;C6</f>
+        <v>Hotkey, %k_comb_backs%, % click_comb_backs</v>
+      </c>
+      <c r="I6" s="8" t="str">
+        <f aca="false">B6&amp;": %k_"&amp;C6&amp;"%"</f>
+        <v>从各子界面返回经营界面: %k_comb_backs%</v>
       </c>
     </row>
   </sheetData>
@@ -1885,4 +3017,120 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="P28:P40 C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.01"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="0" t="str">
+        <f aca="false">A1&amp;", "</f>
+        <v>sub_backs_1, </v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="0" t="str">
+        <f aca="false">A2&amp;", "</f>
+        <v>sub_back_2, </v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">A3&amp;", "</f>
+        <v>sub_back_3, </v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">A4&amp;", "</f>
+        <v>sub_back_build, </v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="0" t="str">
+        <f aca="false">A5&amp;", "</f>
+        <v>sub_back_incident, </v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">A6&amp;", "</f>
+        <v>sub_back_char, </v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="0" t="str">
+        <f aca="false">A7&amp;", "</f>
+        <v>sub_back_building, </v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12页 &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>